<commit_message>
practice exercises with automating the boring stuff with python
</commit_message>
<xml_diff>
--- a/Practice/automate_online-materials/example.xlsx
+++ b/Practice/automate_online-materials/example.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="96" windowWidth="9540" windowHeight="4512"/>
+    <workbookView xWindow="285" yWindow="90" windowWidth="9540" windowHeight="4515"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -39,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,7 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,7 +209,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,19 +384,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E9" sqref="D1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>42099.565300925926</v>
       </c>
@@ -409,7 +407,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>42099.153738425928</v>
       </c>
@@ -420,7 +418,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>42100.532534722224</v>
       </c>
@@ -431,7 +429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>42102.374803240738</v>
       </c>
@@ -442,7 +440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>42104.088194444441</v>
       </c>
@@ -453,7 +451,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>42104.757372685184</v>
       </c>
@@ -464,7 +462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>42104.111643518518</v>
       </c>
@@ -482,24 +480,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>